<commit_message>
Gang spies and percentage spies
</commit_message>
<xml_diff>
--- a/Coursework/PrisonersDilema/Progress.xlsx
+++ b/Coursework/PrisonersDilema/Progress.xlsx
@@ -441,7 +441,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,6 +562,9 @@
       <c r="C10">
         <v>2</v>
       </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -606,11 +609,11 @@
       </c>
       <c r="D14">
         <f>SUM(D2:D13)</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E14" s="2">
         <f>D14/C14</f>
-        <v>0.92</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -634,6 +637,9 @@
       <c r="C17">
         <v>3</v>
       </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
@@ -653,6 +659,9 @@
       <c r="C19">
         <v>2</v>
       </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
@@ -680,6 +689,9 @@
       <c r="C22">
         <v>5</v>
       </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
@@ -713,11 +725,11 @@
       </c>
       <c r="D25">
         <f>SUM(D16:D24)</f>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E25" s="2">
         <f>D25/C25</f>
-        <v>0.48</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
@@ -730,11 +742,11 @@
       </c>
       <c r="D27">
         <f>D14+D25</f>
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E27" s="2">
         <f>D27/C27</f>
-        <v>0.7</v>
+        <v>0.84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>